<commit_message>
new figures and tables
</commit_message>
<xml_diff>
--- a/figures/tables.xlsx
+++ b/figures/tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="414" documentId="13_ncr:1_{0F58EC01-9302-4548-881B-F070D8A116DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{332F6E78-8372-44A6-A44E-0164819200DE}"/>
   <bookViews>
-    <workbookView xWindow="57510" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39370" yWindow="4110" windowWidth="19140" windowHeight="11200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="3" r:id="rId1"/>
@@ -1227,6 +1227,8 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1238,24 +1240,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1278,6 +1262,24 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1293,8 +1295,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1635,17 +1635,17 @@
       <c r="O1" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
@@ -1688,10 +1688,10 @@
       <c r="Y2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="Z2" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="AA2" s="37"/>
+      <c r="AA2" s="39"/>
       <c r="AB2" s="3" t="s">
         <v>89</v>
       </c>
@@ -1939,7 +1939,7 @@
         <f>_xlfn.CONCAT(ROUND(H8,2)," (",ROUND(I8,2),")")</f>
         <v>8.62 (5.58)</v>
       </c>
-      <c r="U8" s="38" t="s">
+      <c r="U8" s="40" t="s">
         <v>46</v>
       </c>
       <c r="V8" s="4" t="s">
@@ -2005,7 +2005,7 @@
         <f>_xlfn.CONCAT(ROUND(H9,2)," (",ROUND(I9,2),")")</f>
         <v>3.18 (4.84)</v>
       </c>
-      <c r="U9" s="38"/>
+      <c r="U9" s="40"/>
       <c r="V9" s="4" t="s">
         <v>15</v>
       </c>
@@ -2069,7 +2069,7 @@
         <f>_xlfn.CONCAT(ROUND(H10,2)," (",ROUND(I10,2),")")</f>
         <v>2.46 (5.89)</v>
       </c>
-      <c r="U10" s="38"/>
+      <c r="U10" s="40"/>
       <c r="V10" s="4" t="s">
         <v>81</v>
       </c>
@@ -2312,7 +2312,7 @@
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="U14" s="38" t="s">
+      <c r="U14" s="40" t="s">
         <v>58</v>
       </c>
       <c r="V14" s="4" t="s">
@@ -2376,7 +2376,7 @@
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="U15" s="38"/>
+      <c r="U15" s="40"/>
       <c r="V15" s="4" t="s">
         <v>35</v>
       </c>
@@ -2726,17 +2726,17 @@
         <f>_xlfn.CONCAT(E21, " (",ROUND(F21,2),")")</f>
         <v>0 (0)</v>
       </c>
-      <c r="U21" s="39" t="s">
+      <c r="U21" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-      <c r="Y21" s="39"/>
-      <c r="Z21" s="39"/>
-      <c r="AA21" s="39"/>
-      <c r="AB21" s="39"/>
-      <c r="AC21" s="39"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41"/>
+      <c r="Z21" s="41"/>
+      <c r="AA21" s="41"/>
+      <c r="AB21" s="41"/>
+      <c r="AC21" s="41"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
@@ -4828,8 +4828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70FBD58-595C-47BD-96EF-9CAED8A98E0F}">
   <dimension ref="A1:AF91"/>
   <sheetViews>
-    <sheetView topLeftCell="L19" workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+    <sheetView tabSelected="1" topLeftCell="R11" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4890,22 +4890,22 @@
       <c r="N1">
         <v>2</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="R1" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
@@ -4953,24 +4953,24 @@
       </c>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
-      <c r="T2" s="43" t="s">
+      <c r="T2" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43" t="s">
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43" t="s">
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
     </row>
     <row r="3" spans="1:32" ht="28" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
@@ -5096,7 +5096,7 @@
         <f t="shared" si="0"/>
         <v>0.21 (0.06, 0.36)</v>
       </c>
-      <c r="R4" s="44" t="s">
+      <c r="R4" s="53" t="s">
         <v>116</v>
       </c>
       <c r="S4" s="12" t="s">
@@ -5175,7 +5175,7 @@
         <f t="shared" si="0"/>
         <v>-1.97 (-2.11, -1.83)</v>
       </c>
-      <c r="R5" s="44"/>
+      <c r="R5" s="53"/>
       <c r="S5" s="12" t="s">
         <v>109</v>
       </c>
@@ -5249,7 +5249,7 @@
         <f t="shared" si="0"/>
         <v>0.01 (-0.08, 0.1)</v>
       </c>
-      <c r="R6" s="44"/>
+      <c r="R6" s="53"/>
       <c r="S6" s="12" t="s">
         <v>105</v>
       </c>
@@ -5323,7 +5323,7 @@
         <f t="shared" si="0"/>
         <v>0.1 (-0.03, 0.24)</v>
       </c>
-      <c r="R7" s="44" t="s">
+      <c r="R7" s="53" t="s">
         <v>102</v>
       </c>
       <c r="S7" s="12" t="s">
@@ -5410,7 +5410,7 @@
         <f t="shared" si="0"/>
         <v>-1.97 (-2.11, -1.83)</v>
       </c>
-      <c r="R8" s="44"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="12" t="s">
         <v>109</v>
       </c>
@@ -5492,7 +5492,7 @@
         <f t="shared" si="0"/>
         <v>0.04 (-0.05, 0.13)</v>
       </c>
-      <c r="R9" s="44"/>
+      <c r="R9" s="53"/>
       <c r="S9" s="12" t="s">
         <v>105</v>
       </c>
@@ -5574,7 +5574,7 @@
         <f t="shared" si="0"/>
         <v>0.13 (-0.01, 0.27)</v>
       </c>
-      <c r="R10" s="44" t="s">
+      <c r="R10" s="53" t="s">
         <v>209</v>
       </c>
       <c r="S10" s="12" t="s">
@@ -5657,7 +5657,7 @@
         <f t="shared" si="0"/>
         <v>-1.96 (-2.06, -1.85)</v>
       </c>
-      <c r="R11" s="44"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="12" t="s">
         <v>109</v>
       </c>
@@ -5735,7 +5735,7 @@
         <f t="shared" si="0"/>
         <v>0.02 (-0.04, 0.09)</v>
       </c>
-      <c r="R12" s="45"/>
+      <c r="R12" s="54"/>
       <c r="S12" s="10" t="s">
         <v>105</v>
       </c>
@@ -5816,22 +5816,22 @@
         <f t="shared" si="0"/>
         <v>0.14 (0.04, 0.24)</v>
       </c>
-      <c r="R13" s="41" t="s">
+      <c r="R13" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
-      <c r="AD13" s="41"/>
-      <c r="AE13" s="41"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="50"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
@@ -6053,18 +6053,18 @@
         <f t="shared" si="0"/>
         <v>0.05 (-0.05, 0.16)</v>
       </c>
-      <c r="Q18" s="42" t="s">
+      <c r="Q18" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
-      <c r="U18" s="42"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="42"/>
-      <c r="X18" s="42"/>
-      <c r="Y18" s="42"/>
-      <c r="Z18" s="42"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
       <c r="AF18" s="8"/>
     </row>
     <row r="19" spans="1:32" ht="42.35" x14ac:dyDescent="0.5">
@@ -6184,10 +6184,10 @@
         <f t="shared" si="0"/>
         <v>-2.39 (-2.55, -2.24)</v>
       </c>
-      <c r="Q20" s="52" t="s">
+      <c r="Q20" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="R20" s="47" t="s">
+      <c r="R20" s="43" t="s">
         <v>102</v>
       </c>
       <c r="S20" s="17" t="s">
@@ -6249,8 +6249,8 @@
         <f t="shared" si="0"/>
         <v>0.09 (-0.11, 0.29)</v>
       </c>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="47"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="43"/>
       <c r="S21" s="17" t="s">
         <v>109</v>
       </c>
@@ -6310,8 +6310,8 @@
         <f t="shared" si="0"/>
         <v>-0.2 (-0.42, 0.02)</v>
       </c>
-      <c r="Q22" s="50"/>
-      <c r="R22" s="47"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="43"/>
       <c r="S22" s="17" t="s">
         <v>105</v>
       </c>
@@ -6374,8 +6374,8 @@
         <f t="shared" si="0"/>
         <v>-1.94 (-2.2, -1.69)</v>
       </c>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="47" t="s">
+      <c r="Q23" s="46"/>
+      <c r="R23" s="43" t="s">
         <v>111</v>
       </c>
       <c r="S23" s="17" t="s">
@@ -6435,8 +6435,8 @@
         <f t="shared" si="0"/>
         <v>-0.13 (-0.24, -0.03)</v>
       </c>
-      <c r="Q24" s="50"/>
-      <c r="R24" s="47"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="43"/>
       <c r="S24" s="17" t="s">
         <v>109</v>
       </c>
@@ -6491,8 +6491,8 @@
         <f t="shared" si="0"/>
         <v>0.03 (-0.15, 0.2)</v>
       </c>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="47"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="43"/>
       <c r="S25" s="17" t="s">
         <v>105</v>
       </c>
@@ -6550,10 +6550,10 @@
         <f t="shared" si="0"/>
         <v>-2.42 (-2.62, -2.21)</v>
       </c>
-      <c r="Q26" s="49" t="s">
+      <c r="Q26" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="R26" s="47" t="s">
+      <c r="R26" s="43" t="s">
         <v>116</v>
       </c>
       <c r="S26" s="17" t="s">
@@ -6616,8 +6616,8 @@
         <f t="shared" si="0"/>
         <v>-0.03 (-0.14, 0.08)</v>
       </c>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="47"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="43"/>
       <c r="S27" s="17" t="s">
         <v>109</v>
       </c>
@@ -6678,8 +6678,8 @@
         <f t="shared" si="0"/>
         <v>-0.17 (-0.35, 0.02)</v>
       </c>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="47"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="43"/>
       <c r="S28" s="17" t="s">
         <v>105</v>
       </c>
@@ -6743,8 +6743,8 @@
         <f t="shared" si="0"/>
         <v>-2.18 (-2.59, -1.78)</v>
       </c>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="47" t="s">
+      <c r="Q29" s="45"/>
+      <c r="R29" s="43" t="s">
         <v>102</v>
       </c>
       <c r="S29" s="17" t="s">
@@ -6810,8 +6810,8 @@
         <f t="shared" si="0"/>
         <v>-0.09 (-0.16, -0.01)</v>
       </c>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="47"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="43"/>
       <c r="S30" s="17" t="s">
         <v>109</v>
       </c>
@@ -6872,8 +6872,8 @@
         <f t="shared" si="0"/>
         <v>-0.06 (-0.19, 0.06)</v>
       </c>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="47"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="43"/>
       <c r="S31" s="17" t="s">
         <v>105</v>
       </c>
@@ -6937,8 +6937,8 @@
         <f t="shared" si="0"/>
         <v>-0.8 (-0.88, -0.71)</v>
       </c>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="47" t="s">
+      <c r="Q32" s="45"/>
+      <c r="R32" s="43" t="s">
         <v>111</v>
       </c>
       <c r="S32" s="17" t="s">
@@ -7001,8 +7001,8 @@
         <f t="shared" si="0"/>
         <v>-0.03 (-0.16, 0.1)</v>
       </c>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="47"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="43"/>
       <c r="S33" s="17" t="s">
         <v>109</v>
       </c>
@@ -7063,8 +7063,8 @@
         <f t="shared" si="0"/>
         <v>-0.02 (-0.14, 0.1)</v>
       </c>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="47"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="43"/>
       <c r="S34" s="17" t="s">
         <v>105</v>
       </c>
@@ -7128,10 +7128,10 @@
         <f t="shared" si="0"/>
         <v>-0.58 (-0.68, -0.48)</v>
       </c>
-      <c r="Q35" s="50" t="s">
+      <c r="Q35" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="R35" s="47" t="s">
+      <c r="R35" s="43" t="s">
         <v>116</v>
       </c>
       <c r="S35" s="17" t="s">
@@ -7194,8 +7194,8 @@
         <f t="shared" si="0"/>
         <v>-0.02 (-0.06, 0.01)</v>
       </c>
-      <c r="Q36" s="50"/>
-      <c r="R36" s="47"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="43"/>
       <c r="S36" s="17" t="s">
         <v>109</v>
       </c>
@@ -7256,8 +7256,8 @@
         <f t="shared" si="0"/>
         <v>-0.02 (-0.07, 0.03)</v>
       </c>
-      <c r="Q37" s="50"/>
-      <c r="R37" s="47"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="43"/>
       <c r="S37" s="17" t="s">
         <v>105</v>
       </c>
@@ -7321,8 +7321,8 @@
         <f t="shared" si="0"/>
         <v>-0.86 (-0.97, -0.75)</v>
       </c>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="47" t="s">
+      <c r="Q38" s="46"/>
+      <c r="R38" s="43" t="s">
         <v>102</v>
       </c>
       <c r="S38" s="17" t="s">
@@ -7387,8 +7387,8 @@
         <f t="shared" si="0"/>
         <v>0 (-0.04, 0.04)</v>
       </c>
-      <c r="Q39" s="50"/>
-      <c r="R39" s="47"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="43"/>
       <c r="S39" s="17" t="s">
         <v>109</v>
       </c>
@@ -7451,8 +7451,8 @@
         <f t="shared" si="0"/>
         <v>0.01 (-0.05, 0.06)</v>
       </c>
-      <c r="Q40" s="50"/>
-      <c r="R40" s="47"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="43"/>
       <c r="S40" s="17" t="s">
         <v>105</v>
       </c>
@@ -7518,8 +7518,8 @@
         <f t="shared" si="0"/>
         <v>-0.72 (-1.02, -0.43)</v>
       </c>
-      <c r="Q41" s="50"/>
-      <c r="R41" s="47" t="s">
+      <c r="Q41" s="46"/>
+      <c r="R41" s="43" t="s">
         <v>111</v>
       </c>
       <c r="S41" s="17" t="s">
@@ -7584,8 +7584,8 @@
         <f t="shared" si="0"/>
         <v>-0.01 (-0.04, 0.01)</v>
       </c>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="47"/>
+      <c r="Q42" s="46"/>
+      <c r="R42" s="43"/>
       <c r="S42" s="17" t="s">
         <v>109</v>
       </c>
@@ -7648,8 +7648,8 @@
         <f t="shared" si="0"/>
         <v>-0.01 (-0.04, 0.03)</v>
       </c>
-      <c r="Q43" s="51"/>
-      <c r="R43" s="48"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="44"/>
       <c r="S43" s="15" t="s">
         <v>105</v>
       </c>
@@ -7715,18 +7715,18 @@
         <f t="shared" si="0"/>
         <v>-2.48 (-2.59, -2.37)</v>
       </c>
-      <c r="Q44" s="46" t="s">
+      <c r="Q44" s="42" t="s">
         <v>270</v>
       </c>
-      <c r="R44" s="46"/>
-      <c r="S44" s="46"/>
-      <c r="T44" s="46"/>
-      <c r="U44" s="46"/>
-      <c r="V44" s="46"/>
-      <c r="W44" s="46"/>
-      <c r="X44" s="46"/>
-      <c r="Y44" s="46"/>
-      <c r="Z44" s="46"/>
+      <c r="R44" s="42"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="42"/>
+      <c r="V44" s="42"/>
+      <c r="W44" s="42"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="42"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
@@ -9830,6 +9830,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="R1:AE1"/>
+    <mergeCell ref="R13:AE13"/>
+    <mergeCell ref="Q18:Z18"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R10:R12"/>
     <mergeCell ref="Q44:Z44"/>
     <mergeCell ref="R20:R22"/>
     <mergeCell ref="R23:R25"/>
@@ -9842,15 +9851,6 @@
     <mergeCell ref="Q26:Q34"/>
     <mergeCell ref="Q35:Q43"/>
     <mergeCell ref="Q20:Q25"/>
-    <mergeCell ref="R1:AE1"/>
-    <mergeCell ref="R13:AE13"/>
-    <mergeCell ref="Q18:Z18"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R10:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9915,13 +9915,13 @@
         <f>_xlfn.CONCAT(D2," (",E2,", ",F2,")")</f>
         <v>-0.33 (-0.512, -0.119)</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="38" t="s">
         <v>245</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
@@ -9946,10 +9946,10 @@
         <f t="shared" ref="H3:H37" si="0">_xlfn.CONCAT(D3," (",E3,", ",F3,")")</f>
         <v>0.041 (-0.199, 0.275)</v>
       </c>
-      <c r="L3" s="53" t="s">
+      <c r="L3" s="55" t="s">
         <v>243</v>
       </c>
-      <c r="M3" s="55" t="s">
+      <c r="M3" s="57" t="s">
         <v>70</v>
       </c>
       <c r="N3" s="3" t="s">
@@ -9985,8 +9985,8 @@
         <f t="shared" si="0"/>
         <v>0.548 (0.355, 0.705)</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="58"/>
       <c r="N4" s="7" t="s">
         <v>56</v>
       </c>
@@ -10020,7 +10020,7 @@
         <f t="shared" si="0"/>
         <v>0.218 (-0.057, 0.465)</v>
       </c>
-      <c r="L5" s="53" t="s">
+      <c r="L5" s="55" t="s">
         <v>265</v>
       </c>
       <c r="M5" s="22" t="s">
@@ -10059,7 +10059,7 @@
         <f t="shared" si="0"/>
         <v>-0.049 (-0.332, 0.252)</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="56"/>
       <c r="M6" s="22" t="s">
         <v>75</v>
       </c>
@@ -10096,7 +10096,7 @@
         <f t="shared" si="0"/>
         <v>-0.448 (-0.658, -0.192)</v>
       </c>
-      <c r="L7" s="54"/>
+      <c r="L7" s="56"/>
       <c r="M7" s="22" t="s">
         <v>76</v>
       </c>
@@ -10133,7 +10133,7 @@
         <f t="shared" si="0"/>
         <v>-0.151 (-0.39, 0.101)</v>
       </c>
-      <c r="L8" s="54"/>
+      <c r="L8" s="56"/>
       <c r="M8" s="22" t="s">
         <v>77</v>
       </c>
@@ -10170,7 +10170,7 @@
         <f t="shared" si="0"/>
         <v>0.064 (-0.193, 0.327)</v>
       </c>
-      <c r="L9" s="54"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="22" t="s">
         <v>78</v>
       </c>
@@ -10207,7 +10207,7 @@
         <f t="shared" si="0"/>
         <v>0.567 (0.377, 0.722)</v>
       </c>
-      <c r="L10" s="54"/>
+      <c r="L10" s="56"/>
       <c r="M10" s="22" t="s">
         <v>79</v>
       </c>
@@ -10273,7 +10273,7 @@
         <f t="shared" si="0"/>
         <v>0.018 (-0.295, 0.335)</v>
       </c>
-      <c r="L12" s="54" t="s">
+      <c r="L12" s="56" t="s">
         <v>244</v>
       </c>
       <c r="M12" s="22" t="s">
@@ -10312,7 +10312,7 @@
         <f t="shared" si="0"/>
         <v>-0.267 (-0.541, 0.038)</v>
       </c>
-      <c r="L13" s="54"/>
+      <c r="L13" s="56"/>
       <c r="M13" s="22" t="s">
         <v>75</v>
       </c>
@@ -10349,7 +10349,7 @@
         <f t="shared" si="0"/>
         <v>-0.222 (-0.373, -0.067)</v>
       </c>
-      <c r="L14" s="54"/>
+      <c r="L14" s="56"/>
       <c r="M14" s="22" t="s">
         <v>76</v>
       </c>
@@ -10386,7 +10386,7 @@
         <f t="shared" si="0"/>
         <v>0.075 (-0.094, 0.244)</v>
       </c>
-      <c r="L15" s="54"/>
+      <c r="L15" s="56"/>
       <c r="M15" s="22" t="s">
         <v>77</v>
       </c>
@@ -10423,7 +10423,7 @@
         <f t="shared" si="0"/>
         <v>0.558 (0.424, 0.67)</v>
       </c>
-      <c r="L16" s="54"/>
+      <c r="L16" s="56"/>
       <c r="M16" s="22" t="s">
         <v>78</v>
       </c>
@@ -10460,7 +10460,7 @@
         <f t="shared" si="0"/>
         <v>0.36 (0.163, 0.538)</v>
       </c>
-      <c r="L17" s="57"/>
+      <c r="L17" s="59"/>
       <c r="M17" s="21" t="s">
         <v>79</v>
       </c>
@@ -10497,13 +10497,13 @@
         <f t="shared" si="0"/>
         <v>-0.034 (-0.248, 0.183)</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="L18" s="41" t="s">
         <v>266</v>
       </c>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
@@ -10978,7 +10978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837D0577-EE48-46BC-BB2C-B27FDF10FE2C}">
   <dimension ref="A2:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B17" sqref="B17:M28"/>
     </sheetView>
   </sheetViews>
@@ -11082,7 +11082,7 @@
       <c r="G5">
         <v>-6.1023429524482502</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="37" t="s">
         <v>289</v>
       </c>
       <c r="I5">
@@ -11478,10 +11478,10 @@
       <c r="H18">
         <v>571</v>
       </c>
-      <c r="I18" s="59" t="s">
+      <c r="I18" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="J18" s="59" t="s">
+      <c r="J18" s="37" t="s">
         <v>293</v>
       </c>
       <c r="K18">
@@ -11516,7 +11516,7 @@
       <c r="H19">
         <v>571</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="I19" s="37" t="s">
         <v>294</v>
       </c>
       <c r="J19">
@@ -11630,7 +11630,7 @@
       <c r="H22">
         <v>571</v>
       </c>
-      <c r="I22" s="59" t="s">
+      <c r="I22" s="37" t="s">
         <v>295</v>
       </c>
       <c r="J22">
@@ -11875,7 +11875,7 @@
       </c>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.5">
-      <c r="H35" s="58"/>
+      <c r="H35" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11886,7 +11886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4096D6E5-B519-4CA2-9221-EBECBC8FA054}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
communication psy partially accepted
</commit_message>
<xml_diff>
--- a/figures/tables.xlsx
+++ b/figures/tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="418" documentId="13_ncr:1_{0F58EC01-9302-4548-881B-F070D8A116DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53925B2E-FAF5-4A0A-A849-593C91BAB98B}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="3" r:id="rId1"/>
@@ -1241,24 +1241,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1279,6 +1261,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A1B876-0218-4255-A060-15655E67617D}">
   <dimension ref="A1:AE87"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="92" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="92" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4890,22 +4890,22 @@
       <c r="N1">
         <v>2</v>
       </c>
-      <c r="R1" s="42" t="s">
+      <c r="R1" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="42"/>
-      <c r="AE1" s="42"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
@@ -4953,24 +4953,24 @@
       </c>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
-      <c r="T2" s="45" t="s">
+      <c r="T2" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45" t="s">
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="45" t="s">
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
     </row>
     <row r="3" spans="1:32" ht="28" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
@@ -5096,7 +5096,7 @@
         <f t="shared" si="0"/>
         <v>0.21 (0.06, 0.36)</v>
       </c>
-      <c r="R4" s="46" t="s">
+      <c r="R4" s="53" t="s">
         <v>115</v>
       </c>
       <c r="S4" s="12" t="s">
@@ -5175,7 +5175,7 @@
         <f t="shared" si="0"/>
         <v>-1.97 (-2.11, -1.83)</v>
       </c>
-      <c r="R5" s="46"/>
+      <c r="R5" s="53"/>
       <c r="S5" s="12" t="s">
         <v>108</v>
       </c>
@@ -5249,7 +5249,7 @@
         <f t="shared" si="0"/>
         <v>0.01 (-0.08, 0.1)</v>
       </c>
-      <c r="R6" s="46"/>
+      <c r="R6" s="53"/>
       <c r="S6" s="12" t="s">
         <v>104</v>
       </c>
@@ -5323,7 +5323,7 @@
         <f t="shared" si="0"/>
         <v>0.1 (-0.03, 0.24)</v>
       </c>
-      <c r="R7" s="46" t="s">
+      <c r="R7" s="53" t="s">
         <v>101</v>
       </c>
       <c r="S7" s="12" t="s">
@@ -5410,7 +5410,7 @@
         <f t="shared" si="0"/>
         <v>-1.97 (-2.11, -1.83)</v>
       </c>
-      <c r="R8" s="46"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="12" t="s">
         <v>108</v>
       </c>
@@ -5492,7 +5492,7 @@
         <f t="shared" si="0"/>
         <v>0.04 (-0.05, 0.13)</v>
       </c>
-      <c r="R9" s="46"/>
+      <c r="R9" s="53"/>
       <c r="S9" s="12" t="s">
         <v>104</v>
       </c>
@@ -5574,7 +5574,7 @@
         <f t="shared" si="0"/>
         <v>0.13 (-0.01, 0.27)</v>
       </c>
-      <c r="R10" s="46" t="s">
+      <c r="R10" s="53" t="s">
         <v>208</v>
       </c>
       <c r="S10" s="12" t="s">
@@ -5657,7 +5657,7 @@
         <f t="shared" si="0"/>
         <v>-1.96 (-2.06, -1.85)</v>
       </c>
-      <c r="R11" s="46"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="12" t="s">
         <v>108</v>
       </c>
@@ -5735,7 +5735,7 @@
         <f t="shared" si="0"/>
         <v>0.02 (-0.04, 0.09)</v>
       </c>
-      <c r="R12" s="47"/>
+      <c r="R12" s="54"/>
       <c r="S12" s="10" t="s">
         <v>104</v>
       </c>
@@ -5816,22 +5816,22 @@
         <f t="shared" si="0"/>
         <v>0.14 (0.04, 0.24)</v>
       </c>
-      <c r="R13" s="43" t="s">
+      <c r="R13" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="43"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="43"/>
-      <c r="AC13" s="43"/>
-      <c r="AD13" s="43"/>
-      <c r="AE13" s="43"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="50"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
@@ -6053,18 +6053,18 @@
         <f t="shared" si="0"/>
         <v>0.05 (-0.05, 0.16)</v>
       </c>
-      <c r="Q18" s="44" t="s">
+      <c r="Q18" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="R18" s="44"/>
-      <c r="S18" s="44"/>
-      <c r="T18" s="44"/>
-      <c r="U18" s="44"/>
-      <c r="V18" s="44"/>
-      <c r="W18" s="44"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="44"/>
-      <c r="Z18" s="44"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
       <c r="AF18" s="8"/>
     </row>
     <row r="19" spans="1:32" ht="42.35" x14ac:dyDescent="0.5">
@@ -6184,10 +6184,10 @@
         <f t="shared" si="0"/>
         <v>-2.39 (-2.55, -2.24)</v>
       </c>
-      <c r="Q20" s="54" t="s">
+      <c r="Q20" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="R20" s="49" t="s">
+      <c r="R20" s="43" t="s">
         <v>101</v>
       </c>
       <c r="S20" s="17" t="s">
@@ -6249,8 +6249,8 @@
         <f t="shared" si="0"/>
         <v>0.09 (-0.11, 0.29)</v>
       </c>
-      <c r="Q21" s="52"/>
-      <c r="R21" s="49"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="43"/>
       <c r="S21" s="17" t="s">
         <v>108</v>
       </c>
@@ -6310,8 +6310,8 @@
         <f t="shared" si="0"/>
         <v>-0.2 (-0.42, 0.02)</v>
       </c>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="49"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="43"/>
       <c r="S22" s="17" t="s">
         <v>104</v>
       </c>
@@ -6374,8 +6374,8 @@
         <f t="shared" si="0"/>
         <v>-1.94 (-2.2, -1.69)</v>
       </c>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="49" t="s">
+      <c r="Q23" s="46"/>
+      <c r="R23" s="43" t="s">
         <v>110</v>
       </c>
       <c r="S23" s="17" t="s">
@@ -6435,8 +6435,8 @@
         <f t="shared" si="0"/>
         <v>-0.13 (-0.24, -0.03)</v>
       </c>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="49"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="43"/>
       <c r="S24" s="17" t="s">
         <v>108</v>
       </c>
@@ -6491,8 +6491,8 @@
         <f t="shared" si="0"/>
         <v>0.03 (-0.15, 0.2)</v>
       </c>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="49"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="43"/>
       <c r="S25" s="17" t="s">
         <v>104</v>
       </c>
@@ -6550,10 +6550,10 @@
         <f t="shared" si="0"/>
         <v>-2.42 (-2.62, -2.21)</v>
       </c>
-      <c r="Q26" s="51" t="s">
+      <c r="Q26" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="R26" s="49" t="s">
+      <c r="R26" s="43" t="s">
         <v>115</v>
       </c>
       <c r="S26" s="17" t="s">
@@ -6616,8 +6616,8 @@
         <f t="shared" si="0"/>
         <v>-0.03 (-0.14, 0.08)</v>
       </c>
-      <c r="Q27" s="51"/>
-      <c r="R27" s="49"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="43"/>
       <c r="S27" s="17" t="s">
         <v>108</v>
       </c>
@@ -6678,8 +6678,8 @@
         <f t="shared" si="0"/>
         <v>-0.17 (-0.35, 0.02)</v>
       </c>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="49"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="43"/>
       <c r="S28" s="17" t="s">
         <v>104</v>
       </c>
@@ -6743,8 +6743,8 @@
         <f t="shared" si="0"/>
         <v>-2.18 (-2.59, -1.78)</v>
       </c>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="49" t="s">
+      <c r="Q29" s="45"/>
+      <c r="R29" s="43" t="s">
         <v>101</v>
       </c>
       <c r="S29" s="17" t="s">
@@ -6810,8 +6810,8 @@
         <f t="shared" si="0"/>
         <v>-0.09 (-0.16, -0.01)</v>
       </c>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="49"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="43"/>
       <c r="S30" s="17" t="s">
         <v>108</v>
       </c>
@@ -6872,8 +6872,8 @@
         <f t="shared" si="0"/>
         <v>-0.06 (-0.19, 0.06)</v>
       </c>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="49"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="43"/>
       <c r="S31" s="17" t="s">
         <v>104</v>
       </c>
@@ -6937,8 +6937,8 @@
         <f t="shared" si="0"/>
         <v>-0.8 (-0.88, -0.71)</v>
       </c>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="49" t="s">
+      <c r="Q32" s="45"/>
+      <c r="R32" s="43" t="s">
         <v>110</v>
       </c>
       <c r="S32" s="17" t="s">
@@ -7001,8 +7001,8 @@
         <f t="shared" si="0"/>
         <v>-0.03 (-0.16, 0.1)</v>
       </c>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="49"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="43"/>
       <c r="S33" s="17" t="s">
         <v>108</v>
       </c>
@@ -7063,8 +7063,8 @@
         <f t="shared" si="0"/>
         <v>-0.02 (-0.14, 0.1)</v>
       </c>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="49"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="43"/>
       <c r="S34" s="17" t="s">
         <v>104</v>
       </c>
@@ -7128,10 +7128,10 @@
         <f t="shared" si="0"/>
         <v>-0.58 (-0.68, -0.48)</v>
       </c>
-      <c r="Q35" s="52" t="s">
+      <c r="Q35" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="R35" s="49" t="s">
+      <c r="R35" s="43" t="s">
         <v>115</v>
       </c>
       <c r="S35" s="17" t="s">
@@ -7194,8 +7194,8 @@
         <f t="shared" si="0"/>
         <v>-0.02 (-0.06, 0.01)</v>
       </c>
-      <c r="Q36" s="52"/>
-      <c r="R36" s="49"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="43"/>
       <c r="S36" s="17" t="s">
         <v>108</v>
       </c>
@@ -7256,8 +7256,8 @@
         <f t="shared" si="0"/>
         <v>-0.02 (-0.07, 0.03)</v>
       </c>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="49"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="43"/>
       <c r="S37" s="17" t="s">
         <v>104</v>
       </c>
@@ -7321,8 +7321,8 @@
         <f t="shared" si="0"/>
         <v>-0.86 (-0.97, -0.75)</v>
       </c>
-      <c r="Q38" s="52"/>
-      <c r="R38" s="49" t="s">
+      <c r="Q38" s="46"/>
+      <c r="R38" s="43" t="s">
         <v>101</v>
       </c>
       <c r="S38" s="17" t="s">
@@ -7387,8 +7387,8 @@
         <f t="shared" si="0"/>
         <v>0 (-0.04, 0.04)</v>
       </c>
-      <c r="Q39" s="52"/>
-      <c r="R39" s="49"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="43"/>
       <c r="S39" s="17" t="s">
         <v>108</v>
       </c>
@@ -7451,8 +7451,8 @@
         <f t="shared" si="0"/>
         <v>0.01 (-0.05, 0.06)</v>
       </c>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="49"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="43"/>
       <c r="S40" s="17" t="s">
         <v>104</v>
       </c>
@@ -7518,8 +7518,8 @@
         <f t="shared" si="0"/>
         <v>-0.72 (-1.02, -0.43)</v>
       </c>
-      <c r="Q41" s="52"/>
-      <c r="R41" s="49" t="s">
+      <c r="Q41" s="46"/>
+      <c r="R41" s="43" t="s">
         <v>110</v>
       </c>
       <c r="S41" s="17" t="s">
@@ -7584,8 +7584,8 @@
         <f t="shared" si="0"/>
         <v>-0.01 (-0.04, 0.01)</v>
       </c>
-      <c r="Q42" s="52"/>
-      <c r="R42" s="49"/>
+      <c r="Q42" s="46"/>
+      <c r="R42" s="43"/>
       <c r="S42" s="17" t="s">
         <v>108</v>
       </c>
@@ -7648,8 +7648,8 @@
         <f t="shared" si="0"/>
         <v>-0.01 (-0.04, 0.03)</v>
       </c>
-      <c r="Q43" s="53"/>
-      <c r="R43" s="50"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="44"/>
       <c r="S43" s="15" t="s">
         <v>104</v>
       </c>
@@ -7715,18 +7715,18 @@
         <f t="shared" si="0"/>
         <v>-2.48 (-2.59, -2.37)</v>
       </c>
-      <c r="Q44" s="48" t="s">
+      <c r="Q44" s="42" t="s">
         <v>269</v>
       </c>
-      <c r="R44" s="48"/>
-      <c r="S44" s="48"/>
-      <c r="T44" s="48"/>
-      <c r="U44" s="48"/>
-      <c r="V44" s="48"/>
-      <c r="W44" s="48"/>
-      <c r="X44" s="48"/>
-      <c r="Y44" s="48"/>
-      <c r="Z44" s="48"/>
+      <c r="R44" s="42"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="42"/>
+      <c r="V44" s="42"/>
+      <c r="W44" s="42"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="42"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
@@ -9830,6 +9830,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="R1:AE1"/>
+    <mergeCell ref="R13:AE13"/>
+    <mergeCell ref="Q18:Z18"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R10:R12"/>
     <mergeCell ref="Q44:Z44"/>
     <mergeCell ref="R20:R22"/>
     <mergeCell ref="R23:R25"/>
@@ -9842,15 +9851,6 @@
     <mergeCell ref="Q26:Q34"/>
     <mergeCell ref="Q35:Q43"/>
     <mergeCell ref="Q20:Q25"/>
-    <mergeCell ref="R1:AE1"/>
-    <mergeCell ref="R13:AE13"/>
-    <mergeCell ref="Q18:Z18"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R10:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9861,7 +9861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6EF612-2EAA-47F0-A461-37A3A32210F7}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="129" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="129" workbookViewId="0">
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>

</xml_diff>